<commit_message>
Updated MOSIP Pending Backlog
</commit_message>
<xml_diff>
--- a/_files/requirements/MOSIP_Backlog_Consolidated.xlsx
+++ b/_files/requirements/MOSIP_Backlog_Consolidated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{292065F0-23CB-49AD-8169-B27104407073}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{983C4B16-A53C-4201-9DA7-D65B23DABDE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" xr2:uid="{DA987513-FE54-4ED6-877C-76611AB6F5C5}"/>
   </bookViews>
@@ -6080,6 +6080,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6093,17 +6102,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6423,10 +6425,10 @@
   <dimension ref="A1:Z585"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="G584" sqref="G584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -6457,11 +6459,11 @@
   <sheetData>
     <row r="1" spans="2:26" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="Z2" s="21"/>
     </row>
     <row r="3" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -10318,7 +10320,7 @@
       <c r="C89" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D89" s="27" t="s">
+      <c r="D89" s="30" t="s">
         <v>155</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -10362,7 +10364,7 @@
       <c r="C90" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D90" s="27"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="12" t="s">
         <v>19</v>
       </c>
@@ -32615,7 +32617,7 @@
       <c r="Y583" s="9"/>
     </row>
     <row r="584" spans="2:25" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B584" s="35">
+      <c r="B584" s="29">
         <v>580</v>
       </c>
       <c r="C584" s="9" t="s">
@@ -32627,10 +32629,10 @@
       <c r="E584" s="26" t="s">
         <v>715</v>
       </c>
-      <c r="F584" s="31" t="s">
+      <c r="F584" s="34" t="s">
         <v>1737</v>
       </c>
-      <c r="G584" s="32" t="s">
+      <c r="G584" s="35" t="s">
         <v>1736</v>
       </c>
       <c r="H584" s="9" t="s">
@@ -32663,14 +32665,14 @@
       <c r="Y584" s="9"/>
     </row>
     <row r="585" spans="2:25" ht="14.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I585" s="33" t="s">
+      <c r="I585" s="27" t="s">
         <v>1738</v>
       </c>
-      <c r="J585" s="34"/>
-      <c r="K585" s="34"/>
-      <c r="L585" s="34"/>
-      <c r="M585" s="34"/>
-      <c r="N585" s="34">
+      <c r="J585" s="28"/>
+      <c r="K585" s="28"/>
+      <c r="L585" s="28"/>
+      <c r="M585" s="28"/>
+      <c r="N585" s="28">
         <f>SUM(N5:N584)</f>
         <v>4220.45</v>
       </c>

</xml_diff>

<commit_message>
reg client estimates are updated
</commit_message>
<xml_diff>
--- a/_files/requirements/MOSIP_Backlog_Consolidated.xlsx
+++ b/_files/requirements/MOSIP_Backlog_Consolidated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF04F44D-178C-453A-A4CE-E0F6EE274D78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6269B6C3-7A67-4C89-8FC0-E52E65452873}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" xr2:uid="{DA987513-FE54-4ED6-877C-76611AB6F5C5}"/>
   </bookViews>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4584" uniqueCount="1741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4586" uniqueCount="1743">
   <si>
     <t>MOSIP - Consolidated Roadmap post 30Jun</t>
   </si>
@@ -5754,6 +5754,12 @@
   </si>
   <si>
     <t>Design, Development, UinitTesting, Manual Testing, Integration</t>
+  </si>
+  <si>
+    <t>To be determined the procedure for this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open JDK is not contians all modules. Need to do the R&amp;D. </t>
   </si>
 </sst>
 </file>
@@ -5993,7 +5999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6074,6 +6080,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6405,13 +6414,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFE7CEB-FADE-4E61-8A23-4DC6C9C8C44B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z586"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="F156" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C439" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="E450" sqref="E450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -6442,11 +6452,11 @@
   <sheetData>
     <row r="1" spans="2:26" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="Z2" s="21"/>
     </row>
     <row r="3" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6526,7 +6536,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="42" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
         <v>1</v>
       </c>
@@ -6568,7 +6578,7 @@
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" spans="2:26" ht="112" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
         <v>2</v>
       </c>
@@ -6618,7 +6628,7 @@
       </c>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" spans="2:26" ht="112" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:26" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -6668,7 +6678,7 @@
       </c>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:26" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -6720,7 +6730,7 @@
       </c>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="2:26" ht="98" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:26" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -6770,7 +6780,7 @@
       </c>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" spans="2:26" ht="98" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:26" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -6822,7 +6832,7 @@
       </c>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="2:26" ht="98" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:26" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
         <v>7</v>
       </c>
@@ -6872,7 +6882,7 @@
       </c>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" spans="2:26" ht="112" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:26" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -6924,7 +6934,7 @@
       </c>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:26" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>9</v>
       </c>
@@ -6974,7 +6984,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="14" spans="2:26" ht="70" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:26" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14" s="7">
         <v>10</v>
       </c>
@@ -7018,7 +7028,7 @@
       </c>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" spans="2:26" ht="56" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:26" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7">
         <v>11</v>
       </c>
@@ -7062,7 +7072,7 @@
       </c>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" spans="2:26" ht="28" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:26" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7">
         <v>12</v>
       </c>
@@ -7104,7 +7114,7 @@
       </c>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
         <v>13</v>
       </c>
@@ -7146,7 +7156,7 @@
       </c>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7">
         <v>14</v>
       </c>
@@ -7186,7 +7196,7 @@
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7">
         <v>15</v>
       </c>
@@ -7228,7 +7238,7 @@
       </c>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
         <v>16</v>
       </c>
@@ -7266,7 +7276,7 @@
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
     </row>
-    <row r="21" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
         <v>17</v>
       </c>
@@ -7306,7 +7316,7 @@
       </c>
       <c r="Y21" s="12"/>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
         <v>18</v>
       </c>
@@ -7454,7 +7464,7 @@
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
     </row>
-    <row r="26" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B26" s="7">
         <v>22</v>
       </c>
@@ -7496,7 +7506,7 @@
       </c>
       <c r="Y26" s="12"/>
     </row>
-    <row r="27" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B27" s="7">
         <v>23</v>
       </c>
@@ -7536,7 +7546,7 @@
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
     </row>
-    <row r="28" spans="2:25" ht="126" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:25" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="B28" s="7">
         <v>24</v>
       </c>
@@ -7578,7 +7588,7 @@
       </c>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7">
         <v>25</v>
       </c>
@@ -7618,7 +7628,7 @@
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
     </row>
-    <row r="30" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30" s="7">
         <v>26</v>
       </c>
@@ -7654,7 +7664,7 @@
       <c r="X30" s="12"/>
       <c r="Y30" s="12"/>
     </row>
-    <row r="31" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31" s="7">
         <v>27</v>
       </c>
@@ -7690,7 +7700,7 @@
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
     </row>
-    <row r="32" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32" s="7">
         <v>28</v>
       </c>
@@ -7732,7 +7742,7 @@
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33" s="7">
         <v>29</v>
       </c>
@@ -7768,7 +7778,7 @@
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
     </row>
-    <row r="34" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34" s="7">
         <v>30</v>
       </c>
@@ -7808,7 +7818,7 @@
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35" s="7">
         <v>31</v>
       </c>
@@ -7930,7 +7940,7 @@
       </c>
       <c r="Y37" s="12"/>
     </row>
-    <row r="38" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38" s="7">
         <v>34</v>
       </c>
@@ -7974,7 +7984,7 @@
       </c>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="2:25" s="16" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:25" s="16" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B39" s="7">
         <v>35</v>
       </c>
@@ -8020,7 +8030,7 @@
       </c>
       <c r="Y39" s="10"/>
     </row>
-    <row r="40" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" s="7">
         <v>36</v>
       </c>
@@ -8066,7 +8076,7 @@
       </c>
       <c r="Y40" s="12"/>
     </row>
-    <row r="41" spans="2:25" ht="140" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:25" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="B41" s="7">
         <v>37</v>
       </c>
@@ -8112,7 +8122,7 @@
       </c>
       <c r="Y41" s="12"/>
     </row>
-    <row r="42" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B42" s="7">
         <v>38</v>
       </c>
@@ -8158,7 +8168,7 @@
       </c>
       <c r="Y42" s="12"/>
     </row>
-    <row r="43" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B43" s="7">
         <v>39</v>
       </c>
@@ -8204,7 +8214,7 @@
       </c>
       <c r="Y43" s="12"/>
     </row>
-    <row r="44" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B44" s="7">
         <v>40</v>
       </c>
@@ -8254,7 +8264,7 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
     </row>
-    <row r="45" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B45" s="7">
         <v>41</v>
       </c>
@@ -8302,7 +8312,7 @@
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
     </row>
-    <row r="46" spans="2:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:25" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="7">
         <v>42</v>
       </c>
@@ -8352,7 +8362,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="2:25" ht="140" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:25" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="B47" s="7">
         <v>43</v>
       </c>
@@ -8398,7 +8408,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="48" spans="2:25" ht="112" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:25" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="B48" s="7">
         <v>44</v>
       </c>
@@ -8442,7 +8452,7 @@
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
     </row>
-    <row r="49" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B49" s="7">
         <v>45</v>
       </c>
@@ -8488,7 +8498,7 @@
       </c>
       <c r="Y49" s="12"/>
     </row>
-    <row r="50" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B50" s="7">
         <v>46</v>
       </c>
@@ -8534,7 +8544,7 @@
       </c>
       <c r="Y50" s="12"/>
     </row>
-    <row r="51" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B51" s="7">
         <v>47</v>
       </c>
@@ -8578,7 +8588,7 @@
       <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
     </row>
-    <row r="52" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B52" s="7">
         <v>48</v>
       </c>
@@ -8624,7 +8634,7 @@
       </c>
       <c r="Y52" s="12"/>
     </row>
-    <row r="53" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B53" s="7">
         <v>49</v>
       </c>
@@ -8672,7 +8682,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="54" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B54" s="7">
         <v>50</v>
       </c>
@@ -8720,7 +8730,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="55" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B55" s="7">
         <v>51</v>
       </c>
@@ -8768,7 +8778,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="56" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B56" s="7">
         <v>52</v>
       </c>
@@ -8866,7 +8876,7 @@
       </c>
       <c r="Y57" s="12"/>
     </row>
-    <row r="58" spans="2:25" ht="140" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:25" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="B58" s="7">
         <v>54</v>
       </c>
@@ -8958,7 +8968,7 @@
       <c r="X59" s="12"/>
       <c r="Y59" s="12"/>
     </row>
-    <row r="60" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B60" s="7">
         <v>56</v>
       </c>
@@ -9002,7 +9012,7 @@
       <c r="X60" s="12"/>
       <c r="Y60" s="12"/>
     </row>
-    <row r="61" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B61" s="7">
         <v>57</v>
       </c>
@@ -9046,7 +9056,7 @@
       <c r="X61" s="12"/>
       <c r="Y61" s="12"/>
     </row>
-    <row r="62" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B62" s="7">
         <v>58</v>
       </c>
@@ -9180,7 +9190,7 @@
       <c r="X64" s="13"/>
       <c r="Y64" s="13"/>
     </row>
-    <row r="65" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B65" s="7">
         <v>61</v>
       </c>
@@ -9228,7 +9238,7 @@
       <c r="X65" s="12"/>
       <c r="Y65" s="12"/>
     </row>
-    <row r="66" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B66" s="7">
         <v>62</v>
       </c>
@@ -9270,7 +9280,7 @@
       <c r="X66" s="12"/>
       <c r="Y66" s="12"/>
     </row>
-    <row r="67" spans="2:25" ht="98" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:25" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B67" s="7">
         <v>63</v>
       </c>
@@ -9312,7 +9322,7 @@
       <c r="X67" s="12"/>
       <c r="Y67" s="12"/>
     </row>
-    <row r="68" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:25" ht="56" x14ac:dyDescent="0.35">
       <c r="B68" s="7">
         <v>64</v>
       </c>
@@ -9362,7 +9372,7 @@
       </c>
       <c r="Y68" s="12"/>
     </row>
-    <row r="69" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69" s="7">
         <v>65</v>
       </c>
@@ -9406,7 +9416,7 @@
       </c>
       <c r="Y69" s="12"/>
     </row>
-    <row r="70" spans="2:25" ht="112" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:25" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70" s="7">
         <v>66</v>
       </c>
@@ -9450,7 +9460,7 @@
       </c>
       <c r="Y70" s="12"/>
     </row>
-    <row r="71" spans="2:25" ht="140" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:25" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="B71" s="7">
         <v>67</v>
       </c>
@@ -9494,7 +9504,7 @@
       </c>
       <c r="Y71" s="12"/>
     </row>
-    <row r="72" spans="2:25" ht="126" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:25" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="B72" s="7">
         <v>68</v>
       </c>
@@ -9536,7 +9546,7 @@
       <c r="X72" s="12"/>
       <c r="Y72" s="12"/>
     </row>
-    <row r="73" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73" s="7">
         <v>69</v>
       </c>
@@ -9578,7 +9588,7 @@
       <c r="X73" s="12"/>
       <c r="Y73" s="12"/>
     </row>
-    <row r="74" spans="2:25" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:25" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="7">
         <v>70</v>
       </c>
@@ -9622,7 +9632,7 @@
       </c>
       <c r="Y74" s="4"/>
     </row>
-    <row r="75" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75" s="7">
         <v>71</v>
       </c>
@@ -9666,7 +9676,7 @@
       </c>
       <c r="Y75" s="12"/>
     </row>
-    <row r="76" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B76" s="7">
         <v>72</v>
       </c>
@@ -10158,7 +10168,7 @@
       </c>
       <c r="Y85" s="12"/>
     </row>
-    <row r="86" spans="2:25" ht="196" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:25" ht="196" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86" s="7">
         <v>82</v>
       </c>
@@ -10252,7 +10262,7 @@
       </c>
       <c r="Y87" s="12"/>
     </row>
-    <row r="88" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88" s="7">
         <v>84</v>
       </c>
@@ -10296,14 +10306,14 @@
       </c>
       <c r="Y88" s="12"/>
     </row>
-    <row r="89" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B89" s="7">
         <v>85</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D89" s="29" t="s">
+      <c r="D89" s="30" t="s">
         <v>155</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -10340,14 +10350,14 @@
       </c>
       <c r="Y89" s="12"/>
     </row>
-    <row r="90" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B90" s="7">
         <v>86</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D90" s="29"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="12" t="s">
         <v>19</v>
       </c>
@@ -10382,7 +10392,7 @@
       </c>
       <c r="Y90" s="12"/>
     </row>
-    <row r="91" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B91" s="7">
         <v>87</v>
       </c>
@@ -10426,7 +10436,7 @@
       </c>
       <c r="Y91" s="12"/>
     </row>
-    <row r="92" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B92" s="7">
         <v>88</v>
       </c>
@@ -10470,7 +10480,7 @@
       </c>
       <c r="Y92" s="12"/>
     </row>
-    <row r="93" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B93" s="7">
         <v>89</v>
       </c>
@@ -10514,7 +10524,7 @@
       </c>
       <c r="Y93" s="12"/>
     </row>
-    <row r="94" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B94" s="7">
         <v>90</v>
       </c>
@@ -10566,7 +10576,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="95" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95" s="7">
         <v>91</v>
       </c>
@@ -10610,7 +10620,7 @@
       </c>
       <c r="Y95" s="12"/>
     </row>
-    <row r="96" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96" s="7">
         <v>92</v>
       </c>
@@ -10652,7 +10662,7 @@
       <c r="X96" s="12"/>
       <c r="Y96" s="12"/>
     </row>
-    <row r="97" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97" s="7">
         <v>93</v>
       </c>
@@ -10744,7 +10754,7 @@
       <c r="X98" s="12"/>
       <c r="Y98" s="12"/>
     </row>
-    <row r="99" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B99" s="7">
         <v>95</v>
       </c>
@@ -10790,7 +10800,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="100" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B100" s="7">
         <v>96</v>
       </c>
@@ -10834,7 +10844,7 @@
       </c>
       <c r="Y100" s="12"/>
     </row>
-    <row r="101" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B101" s="7">
         <v>97</v>
       </c>
@@ -10878,7 +10888,7 @@
       </c>
       <c r="Y101" s="12"/>
     </row>
-    <row r="102" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B102" s="7">
         <v>98</v>
       </c>
@@ -10924,7 +10934,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="103" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B103" s="7">
         <v>99</v>
       </c>
@@ -10968,7 +10978,7 @@
       </c>
       <c r="Y103" s="6"/>
     </row>
-    <row r="104" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B104" s="7">
         <v>100</v>
       </c>
@@ -11012,7 +11022,7 @@
       </c>
       <c r="Y104" s="6"/>
     </row>
-    <row r="105" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B105" s="7">
         <v>101</v>
       </c>
@@ -11056,7 +11066,7 @@
       </c>
       <c r="Y105" s="6"/>
     </row>
-    <row r="106" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B106" s="7">
         <v>102</v>
       </c>
@@ -11098,7 +11108,7 @@
       <c r="X106" s="12"/>
       <c r="Y106" s="12"/>
     </row>
-    <row r="107" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B107" s="7">
         <v>103</v>
       </c>
@@ -11146,7 +11156,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="108" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B108" s="7">
         <v>104</v>
       </c>
@@ -11194,7 +11204,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="109" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B109" s="7">
         <v>105</v>
       </c>
@@ -11242,7 +11252,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="110" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B110" s="7">
         <v>106</v>
       </c>
@@ -11290,7 +11300,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="111" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B111" s="7">
         <v>107</v>
       </c>
@@ -11338,7 +11348,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="112" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B112" s="7">
         <v>108</v>
       </c>
@@ -11386,7 +11396,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="113" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B113" s="7">
         <v>109</v>
       </c>
@@ -11434,7 +11444,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="114" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B114" s="7">
         <v>110</v>
       </c>
@@ -11482,7 +11492,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="115" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B115" s="7">
         <v>111</v>
       </c>
@@ -11584,7 +11594,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="117" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B117" s="7">
         <v>113</v>
       </c>
@@ -11632,7 +11642,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="118" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B118" s="7">
         <v>114</v>
       </c>
@@ -11680,7 +11690,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="119" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B119" s="7">
         <v>115</v>
       </c>
@@ -11728,7 +11738,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="120" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B120" s="7">
         <v>116</v>
       </c>
@@ -11776,7 +11786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B121" s="7">
         <v>117</v>
       </c>
@@ -11824,7 +11834,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="122" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B122" s="7">
         <v>118</v>
       </c>
@@ -11870,7 +11880,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="123" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B123" s="7">
         <v>119</v>
       </c>
@@ -11918,7 +11928,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="124" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B124" s="7">
         <v>120</v>
       </c>
@@ -11966,7 +11976,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="125" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B125" s="7">
         <v>121</v>
       </c>
@@ -12014,7 +12024,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="126" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B126" s="7">
         <v>122</v>
       </c>
@@ -12068,7 +12078,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="127" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B127" s="7">
         <v>123</v>
       </c>
@@ -12118,7 +12128,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="128" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B128" s="7">
         <v>124</v>
       </c>
@@ -12166,7 +12176,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="129" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B129" s="7">
         <v>125</v>
       </c>
@@ -12214,7 +12224,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="130" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B130" s="7">
         <v>126</v>
       </c>
@@ -12262,7 +12272,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="131" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B131" s="7">
         <v>127</v>
       </c>
@@ -12310,7 +12320,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="132" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B132" s="7">
         <v>128</v>
       </c>
@@ -12358,7 +12368,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="133" spans="2:25" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:25" ht="52" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B133" s="7">
         <v>129</v>
       </c>
@@ -12408,7 +12418,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="134" spans="2:25" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:25" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B134" s="7">
         <v>130</v>
       </c>
@@ -12450,7 +12460,7 @@
       <c r="X134" s="12"/>
       <c r="Y134" s="12"/>
     </row>
-    <row r="135" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B135" s="7">
         <v>131</v>
       </c>
@@ -12494,7 +12504,7 @@
       <c r="X135" s="12"/>
       <c r="Y135" s="12"/>
     </row>
-    <row r="136" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B136" s="7">
         <v>132</v>
       </c>
@@ -12571,7 +12581,9 @@
         <v>679</v>
       </c>
       <c r="M137" s="12"/>
-      <c r="N137" s="12"/>
+      <c r="N137" s="12">
+        <v>10</v>
+      </c>
       <c r="O137" s="12"/>
       <c r="P137" s="12"/>
       <c r="Q137" s="12"/>
@@ -12584,7 +12596,7 @@
       <c r="X137" s="12"/>
       <c r="Y137" s="12"/>
     </row>
-    <row r="138" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B138" s="7">
         <v>134</v>
       </c>
@@ -12659,7 +12671,9 @@
         <v>679</v>
       </c>
       <c r="M139" s="12"/>
-      <c r="N139" s="12"/>
+      <c r="N139" s="12">
+        <v>10</v>
+      </c>
       <c r="O139" s="12"/>
       <c r="P139" s="12"/>
       <c r="Q139" s="12"/>
@@ -12672,7 +12686,7 @@
       <c r="X139" s="12"/>
       <c r="Y139" s="12"/>
     </row>
-    <row r="140" spans="2:25" ht="182" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:25" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="B140" s="7">
         <v>136</v>
       </c>
@@ -12751,7 +12765,9 @@
       <c r="M141" s="12" t="s">
         <v>718</v>
       </c>
-      <c r="N141" s="12"/>
+      <c r="N141" s="12">
+        <v>30</v>
+      </c>
       <c r="O141" s="12"/>
       <c r="P141" s="12"/>
       <c r="Q141" s="12"/>
@@ -12797,7 +12813,9 @@
       <c r="M142" s="12" t="s">
         <v>345</v>
       </c>
-      <c r="N142" s="12"/>
+      <c r="N142" s="12">
+        <v>20</v>
+      </c>
       <c r="O142" s="12"/>
       <c r="P142" s="12"/>
       <c r="Q142" s="12"/>
@@ -12839,7 +12857,9 @@
       </c>
       <c r="L143" s="12"/>
       <c r="M143" s="12"/>
-      <c r="N143" s="12"/>
+      <c r="N143" s="12">
+        <v>20</v>
+      </c>
       <c r="O143" s="12"/>
       <c r="P143" s="12"/>
       <c r="Q143" s="12"/>
@@ -12885,7 +12905,9 @@
       <c r="M144" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="N144" s="12"/>
+      <c r="N144" s="12">
+        <v>20</v>
+      </c>
       <c r="O144" s="12"/>
       <c r="P144" s="12"/>
       <c r="Q144" s="12"/>
@@ -12931,7 +12953,9 @@
       <c r="M145" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="N145" s="12"/>
+      <c r="N145" s="12">
+        <v>20</v>
+      </c>
       <c r="O145" s="12"/>
       <c r="P145" s="12"/>
       <c r="Q145" s="12"/>
@@ -12975,7 +12999,9 @@
       <c r="M146" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N146" s="12"/>
+      <c r="N146" s="12">
+        <v>20</v>
+      </c>
       <c r="O146" s="12"/>
       <c r="P146" s="12"/>
       <c r="Q146" s="12"/>
@@ -13029,7 +13055,9 @@
       <c r="U147" s="12"/>
       <c r="V147" s="12"/>
       <c r="W147" s="12"/>
-      <c r="X147" s="12"/>
+      <c r="X147" s="29" t="s">
+        <v>1741</v>
+      </c>
       <c r="Y147" s="12"/>
     </row>
     <row r="148" spans="2:25" ht="28" x14ac:dyDescent="0.35">
@@ -13059,7 +13087,9 @@
       </c>
       <c r="L148" s="13"/>
       <c r="M148" s="13"/>
-      <c r="N148" s="13"/>
+      <c r="N148" s="13">
+        <v>200</v>
+      </c>
       <c r="O148" s="13"/>
       <c r="P148" s="13"/>
       <c r="Q148" s="13"/>
@@ -13069,7 +13099,9 @@
       <c r="U148" s="13"/>
       <c r="V148" s="13"/>
       <c r="W148" s="13"/>
-      <c r="X148" s="13"/>
+      <c r="X148" s="29" t="s">
+        <v>1742</v>
+      </c>
       <c r="Y148" s="13"/>
     </row>
     <row r="149" spans="2:25" ht="28" x14ac:dyDescent="0.35">
@@ -13101,7 +13133,9 @@
       <c r="M149" s="25" t="s">
         <v>1728</v>
       </c>
-      <c r="N149" s="13"/>
+      <c r="N149" s="13">
+        <v>30</v>
+      </c>
       <c r="O149" s="13"/>
       <c r="P149" s="13"/>
       <c r="Q149" s="13"/>
@@ -13145,7 +13179,9 @@
       </c>
       <c r="L150" s="13"/>
       <c r="M150" s="13"/>
-      <c r="N150" s="13"/>
+      <c r="N150" s="13">
+        <v>30</v>
+      </c>
       <c r="O150" s="13"/>
       <c r="P150" s="13"/>
       <c r="Q150" s="13"/>
@@ -13158,7 +13194,7 @@
       <c r="X150" s="13"/>
       <c r="Y150" s="13"/>
     </row>
-    <row r="151" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B151" s="7">
         <v>147</v>
       </c>
@@ -13202,7 +13238,7 @@
       <c r="X151" s="12"/>
       <c r="Y151" s="12"/>
     </row>
-    <row r="152" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B152" s="7">
         <v>148</v>
       </c>
@@ -13246,7 +13282,7 @@
       <c r="X152" s="12"/>
       <c r="Y152" s="12"/>
     </row>
-    <row r="153" spans="2:25" ht="126" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:25" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="B153" s="7">
         <v>149</v>
       </c>
@@ -13292,7 +13328,7 @@
       </c>
       <c r="Y153" s="12"/>
     </row>
-    <row r="154" spans="2:25" ht="266" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:25" ht="266" hidden="1" x14ac:dyDescent="0.35">
       <c r="B154" s="7">
         <v>150</v>
       </c>
@@ -13340,7 +13376,7 @@
       </c>
       <c r="Y154" s="12"/>
     </row>
-    <row r="155" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B155" s="7">
         <v>151</v>
       </c>
@@ -13438,7 +13474,7 @@
       </c>
       <c r="Y156" s="12"/>
     </row>
-    <row r="157" spans="2:25" ht="98" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:25" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B157" s="7">
         <v>153</v>
       </c>
@@ -13484,7 +13520,7 @@
       </c>
       <c r="Y157" s="12"/>
     </row>
-    <row r="158" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B158" s="7">
         <v>154</v>
       </c>
@@ -13580,7 +13616,7 @@
       </c>
       <c r="Y159" s="12"/>
     </row>
-    <row r="160" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B160" s="7">
         <v>156</v>
       </c>
@@ -13624,7 +13660,7 @@
       <c r="X160" s="12"/>
       <c r="Y160" s="12"/>
     </row>
-    <row r="161" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B161" s="7">
         <v>157</v>
       </c>
@@ -13668,7 +13704,7 @@
       <c r="X161" s="12"/>
       <c r="Y161" s="12"/>
     </row>
-    <row r="162" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B162" s="7">
         <v>158</v>
       </c>
@@ -13714,7 +13750,7 @@
       </c>
       <c r="Y162" s="12"/>
     </row>
-    <row r="163" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B163" s="7">
         <v>159</v>
       </c>
@@ -13758,7 +13794,7 @@
       <c r="X163" s="12"/>
       <c r="Y163" s="12"/>
     </row>
-    <row r="164" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B164" s="7">
         <v>160</v>
       </c>
@@ -13802,7 +13838,7 @@
       <c r="X164" s="4"/>
       <c r="Y164" s="4"/>
     </row>
-    <row r="165" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B165" s="7">
         <v>161</v>
       </c>
@@ -13846,7 +13882,7 @@
       <c r="X165" s="12"/>
       <c r="Y165" s="12"/>
     </row>
-    <row r="166" spans="2:25" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:25" ht="72.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B166" s="7">
         <v>162</v>
       </c>
@@ -13940,7 +13976,7 @@
       </c>
       <c r="Y167" s="12"/>
     </row>
-    <row r="168" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B168" s="7">
         <v>164</v>
       </c>
@@ -13986,7 +14022,7 @@
       </c>
       <c r="Y168" s="12"/>
     </row>
-    <row r="169" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B169" s="7">
         <v>165</v>
       </c>
@@ -14032,7 +14068,7 @@
       </c>
       <c r="Y169" s="12"/>
     </row>
-    <row r="170" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B170" s="7">
         <v>166</v>
       </c>
@@ -14228,7 +14264,7 @@
       </c>
       <c r="Y173" s="12"/>
     </row>
-    <row r="174" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B174" s="7">
         <v>170</v>
       </c>
@@ -15194,7 +15230,7 @@
       <c r="X193" s="13"/>
       <c r="Y193" s="13"/>
     </row>
-    <row r="194" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B194" s="7">
         <v>190</v>
       </c>
@@ -15292,7 +15328,7 @@
       <c r="X195" s="12"/>
       <c r="Y195" s="12"/>
     </row>
-    <row r="196" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="196" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B196" s="7">
         <v>192</v>
       </c>
@@ -15342,7 +15378,7 @@
       </c>
       <c r="Y196" s="12"/>
     </row>
-    <row r="197" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B197" s="7">
         <v>193</v>
       </c>
@@ -15842,7 +15878,7 @@
       <c r="X206" s="12"/>
       <c r="Y206" s="12"/>
     </row>
-    <row r="207" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="207" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B207" s="7">
         <v>203</v>
       </c>
@@ -15888,7 +15924,7 @@
       <c r="X207" s="12"/>
       <c r="Y207" s="12"/>
     </row>
-    <row r="208" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="208" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B208" s="7">
         <v>204</v>
       </c>
@@ -15934,7 +15970,7 @@
       <c r="X208" s="12"/>
       <c r="Y208" s="12"/>
     </row>
-    <row r="209" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="209" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B209" s="7">
         <v>205</v>
       </c>
@@ -15980,7 +16016,7 @@
       </c>
       <c r="Y209" s="12"/>
     </row>
-    <row r="210" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="210" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B210" s="7">
         <v>206</v>
       </c>
@@ -16026,7 +16062,7 @@
       </c>
       <c r="Y210" s="12"/>
     </row>
-    <row r="211" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="211" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B211" s="7">
         <v>207</v>
       </c>
@@ -16078,7 +16114,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="212" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="212" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B212" s="7">
         <v>208</v>
       </c>
@@ -16124,7 +16160,7 @@
       <c r="X212" s="12"/>
       <c r="Y212" s="12"/>
     </row>
-    <row r="213" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="213" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B213" s="7">
         <v>209</v>
       </c>
@@ -16224,7 +16260,7 @@
       </c>
       <c r="Y214" s="12"/>
     </row>
-    <row r="215" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="215" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B215" s="7">
         <v>211</v>
       </c>
@@ -16326,7 +16362,7 @@
       </c>
       <c r="Y216" s="12"/>
     </row>
-    <row r="217" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="217" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B217" s="7">
         <v>213</v>
       </c>
@@ -16372,7 +16408,7 @@
       <c r="X217" s="12"/>
       <c r="Y217" s="12"/>
     </row>
-    <row r="218" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="218" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B218" s="7">
         <v>214</v>
       </c>
@@ -16418,7 +16454,7 @@
       <c r="X218" s="12"/>
       <c r="Y218" s="12"/>
     </row>
-    <row r="219" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="219" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B219" s="7">
         <v>215</v>
       </c>
@@ -16464,7 +16500,7 @@
       <c r="X219" s="12"/>
       <c r="Y219" s="12"/>
     </row>
-    <row r="220" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="220" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B220" s="7">
         <v>216</v>
       </c>
@@ -16664,7 +16700,7 @@
       <c r="X223" s="12"/>
       <c r="Y223" s="12"/>
     </row>
-    <row r="224" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="224" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B224" s="7">
         <v>220</v>
       </c>
@@ -16714,7 +16750,7 @@
       </c>
       <c r="Y224" s="12"/>
     </row>
-    <row r="225" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="225" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B225" s="7">
         <v>221</v>
       </c>
@@ -16764,7 +16800,7 @@
       <c r="X225" s="12"/>
       <c r="Y225" s="12"/>
     </row>
-    <row r="226" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="226" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B226" s="7">
         <v>222</v>
       </c>
@@ -16814,7 +16850,7 @@
       </c>
       <c r="Y226" s="12"/>
     </row>
-    <row r="227" spans="2:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="2:25" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B227" s="7">
         <v>223</v>
       </c>
@@ -16858,7 +16894,7 @@
       <c r="X227" s="12"/>
       <c r="Y227" s="12"/>
     </row>
-    <row r="228" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="228" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B228" s="7">
         <v>224</v>
       </c>
@@ -16902,7 +16938,7 @@
       <c r="X228" s="12"/>
       <c r="Y228" s="12"/>
     </row>
-    <row r="229" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="229" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B229" s="7">
         <v>225</v>
       </c>
@@ -16946,7 +16982,7 @@
       <c r="X229" s="12"/>
       <c r="Y229" s="12"/>
     </row>
-    <row r="230" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="230" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B230" s="7">
         <v>226</v>
       </c>
@@ -16996,7 +17032,7 @@
       </c>
       <c r="Y230" s="12"/>
     </row>
-    <row r="231" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="231" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B231" s="7">
         <v>227</v>
       </c>
@@ -17044,7 +17080,7 @@
       <c r="X231" s="12"/>
       <c r="Y231" s="12"/>
     </row>
-    <row r="232" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="232" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B232" s="7">
         <v>228</v>
       </c>
@@ -17092,7 +17128,7 @@
       <c r="X232" s="12"/>
       <c r="Y232" s="12"/>
     </row>
-    <row r="233" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="233" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B233" s="7">
         <v>229</v>
       </c>
@@ -17142,7 +17178,7 @@
       <c r="X233" s="12"/>
       <c r="Y233" s="12"/>
     </row>
-    <row r="234" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="234" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B234" s="7">
         <v>230</v>
       </c>
@@ -17240,7 +17276,7 @@
       <c r="X235" s="12"/>
       <c r="Y235" s="12"/>
     </row>
-    <row r="236" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="236" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B236" s="7">
         <v>232</v>
       </c>
@@ -17286,7 +17322,7 @@
       <c r="X236" s="12"/>
       <c r="Y236" s="12"/>
     </row>
-    <row r="237" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="237" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B237" s="7">
         <v>233</v>
       </c>
@@ -17698,7 +17734,7 @@
       <c r="X245" s="12"/>
       <c r="Y245" s="12"/>
     </row>
-    <row r="246" spans="2:25" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:25" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="B246" s="7">
         <v>242</v>
       </c>
@@ -17850,7 +17886,7 @@
       </c>
       <c r="Y248" s="12"/>
     </row>
-    <row r="249" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B249" s="7">
         <v>245</v>
       </c>
@@ -18196,7 +18232,7 @@
       <c r="X256" s="13"/>
       <c r="Y256" s="13"/>
     </row>
-    <row r="257" spans="1:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B257" s="7">
         <v>253</v>
       </c>
@@ -18396,7 +18432,7 @@
       </c>
       <c r="Y260" s="12"/>
     </row>
-    <row r="261" spans="1:25" s="16" customFormat="1" ht="70" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:25" s="16" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B261" s="7">
         <v>257</v>
       </c>
@@ -18446,7 +18482,7 @@
       </c>
       <c r="Y261" s="10"/>
     </row>
-    <row r="262" spans="1:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" s="16"/>
       <c r="B262" s="7">
         <v>258</v>
@@ -18497,7 +18533,7 @@
       </c>
       <c r="Y262" s="12"/>
     </row>
-    <row r="263" spans="1:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B263" s="7">
         <v>259</v>
       </c>
@@ -18547,7 +18583,7 @@
       </c>
       <c r="Y263" s="12"/>
     </row>
-    <row r="264" spans="1:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B264" s="7">
         <v>260</v>
       </c>
@@ -19033,7 +19069,7 @@
       <c r="X273" s="13"/>
       <c r="Y273" s="13"/>
     </row>
-    <row r="274" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="274" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B274" s="7">
         <v>270</v>
       </c>
@@ -19073,7 +19109,7 @@
       </c>
       <c r="Y274" s="12"/>
     </row>
-    <row r="275" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="275" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B275" s="7">
         <v>271</v>
       </c>
@@ -19113,7 +19149,7 @@
       </c>
       <c r="Y275" s="12"/>
     </row>
-    <row r="276" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="276" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B276" s="7">
         <v>272</v>
       </c>
@@ -19153,7 +19189,7 @@
       </c>
       <c r="Y276" s="12"/>
     </row>
-    <row r="277" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="277" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B277" s="7">
         <v>273</v>
       </c>
@@ -19193,7 +19229,7 @@
       </c>
       <c r="Y277" s="12"/>
     </row>
-    <row r="278" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="278" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B278" s="7">
         <v>274</v>
       </c>
@@ -19233,7 +19269,7 @@
       </c>
       <c r="Y278" s="12"/>
     </row>
-    <row r="279" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="279" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B279" s="7">
         <v>275</v>
       </c>
@@ -19273,7 +19309,7 @@
       </c>
       <c r="Y279" s="12"/>
     </row>
-    <row r="280" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="280" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B280" s="7">
         <v>276</v>
       </c>
@@ -19317,7 +19353,7 @@
       </c>
       <c r="Y280" s="12"/>
     </row>
-    <row r="281" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="281" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B281" s="7">
         <v>277</v>
       </c>
@@ -19357,7 +19393,7 @@
       </c>
       <c r="Y281" s="12"/>
     </row>
-    <row r="282" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="282" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B282" s="7">
         <v>278</v>
       </c>
@@ -19397,7 +19433,7 @@
       </c>
       <c r="Y282" s="12"/>
     </row>
-    <row r="283" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="283" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B283" s="7">
         <v>279</v>
       </c>
@@ -19439,7 +19475,7 @@
       </c>
       <c r="Y283" s="12"/>
     </row>
-    <row r="284" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="284" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B284" s="7">
         <v>280</v>
       </c>
@@ -19481,7 +19517,7 @@
       </c>
       <c r="Y284" s="12"/>
     </row>
-    <row r="285" spans="2:25" ht="112" x14ac:dyDescent="0.35">
+    <row r="285" spans="2:25" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="B285" s="7">
         <v>281</v>
       </c>
@@ -19531,7 +19567,7 @@
       </c>
       <c r="Y285" s="12"/>
     </row>
-    <row r="286" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="286" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B286" s="7">
         <v>282</v>
       </c>
@@ -19573,7 +19609,7 @@
       </c>
       <c r="Y286" s="12"/>
     </row>
-    <row r="287" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="287" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B287" s="7">
         <v>283</v>
       </c>
@@ -19613,7 +19649,7 @@
       </c>
       <c r="Y287" s="12"/>
     </row>
-    <row r="288" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="288" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B288" s="7">
         <v>284</v>
       </c>
@@ -19663,7 +19699,7 @@
       </c>
       <c r="Y288" s="12"/>
     </row>
-    <row r="289" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="289" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B289" s="7">
         <v>285</v>
       </c>
@@ -19709,7 +19745,7 @@
       </c>
       <c r="Y289" s="12"/>
     </row>
-    <row r="290" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="290" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B290" s="7">
         <v>286</v>
       </c>
@@ -19749,7 +19785,7 @@
       </c>
       <c r="Y290" s="12"/>
     </row>
-    <row r="291" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="291" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B291" s="7">
         <v>287</v>
       </c>
@@ -19789,7 +19825,7 @@
       </c>
       <c r="Y291" s="12"/>
     </row>
-    <row r="292" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="292" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B292" s="7">
         <v>288</v>
       </c>
@@ -19831,7 +19867,7 @@
       </c>
       <c r="Y292" s="12"/>
     </row>
-    <row r="293" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="293" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B293" s="7">
         <v>289</v>
       </c>
@@ -19877,7 +19913,7 @@
       </c>
       <c r="Y293" s="12"/>
     </row>
-    <row r="294" spans="2:25" ht="182" x14ac:dyDescent="0.35">
+    <row r="294" spans="2:25" ht="182" hidden="1" x14ac:dyDescent="0.35">
       <c r="B294" s="7">
         <v>290</v>
       </c>
@@ -19927,7 +19963,7 @@
       </c>
       <c r="Y294" s="12"/>
     </row>
-    <row r="295" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="295" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B295" s="7">
         <v>291</v>
       </c>
@@ -19967,7 +20003,7 @@
       </c>
       <c r="Y295" s="12"/>
     </row>
-    <row r="296" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="296" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B296" s="7">
         <v>292</v>
       </c>
@@ -20007,7 +20043,7 @@
       </c>
       <c r="Y296" s="12"/>
     </row>
-    <row r="297" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="297" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B297" s="7">
         <v>293</v>
       </c>
@@ -20047,7 +20083,7 @@
       </c>
       <c r="Y297" s="12"/>
     </row>
-    <row r="298" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="298" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B298" s="7">
         <v>294</v>
       </c>
@@ -20087,7 +20123,7 @@
       </c>
       <c r="Y298" s="12"/>
     </row>
-    <row r="299" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="299" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B299" s="7">
         <v>295</v>
       </c>
@@ -20127,7 +20163,7 @@
       </c>
       <c r="Y299" s="12"/>
     </row>
-    <row r="300" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="300" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B300" s="7">
         <v>296</v>
       </c>
@@ -20167,7 +20203,7 @@
       </c>
       <c r="Y300" s="12"/>
     </row>
-    <row r="301" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="301" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B301" s="7">
         <v>297</v>
       </c>
@@ -20207,7 +20243,7 @@
       </c>
       <c r="Y301" s="12"/>
     </row>
-    <row r="302" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="302" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B302" s="7">
         <v>298</v>
       </c>
@@ -20249,7 +20285,7 @@
       </c>
       <c r="Y302" s="12"/>
     </row>
-    <row r="303" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="303" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B303" s="7">
         <v>299</v>
       </c>
@@ -20291,7 +20327,7 @@
       </c>
       <c r="Y303" s="12"/>
     </row>
-    <row r="304" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="304" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B304" s="7">
         <v>300</v>
       </c>
@@ -20333,7 +20369,7 @@
       </c>
       <c r="Y304" s="12"/>
     </row>
-    <row r="305" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="305" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B305" s="7">
         <v>301</v>
       </c>
@@ -20375,7 +20411,7 @@
       </c>
       <c r="Y305" s="12"/>
     </row>
-    <row r="306" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="306" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B306" s="7">
         <v>302</v>
       </c>
@@ -20417,7 +20453,7 @@
       </c>
       <c r="Y306" s="12"/>
     </row>
-    <row r="307" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="307" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B307" s="7">
         <v>303</v>
       </c>
@@ -20457,7 +20493,7 @@
       </c>
       <c r="Y307" s="12"/>
     </row>
-    <row r="308" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="308" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B308" s="7">
         <v>304</v>
       </c>
@@ -20497,7 +20533,7 @@
       </c>
       <c r="Y308" s="12"/>
     </row>
-    <row r="309" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="309" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B309" s="7">
         <v>305</v>
       </c>
@@ -20535,7 +20571,7 @@
       </c>
       <c r="Y309" s="12"/>
     </row>
-    <row r="310" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="310" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B310" s="7">
         <v>306</v>
       </c>
@@ -20573,7 +20609,7 @@
       </c>
       <c r="Y310" s="12"/>
     </row>
-    <row r="311" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="311" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B311" s="7">
         <v>307</v>
       </c>
@@ -20611,7 +20647,7 @@
       </c>
       <c r="Y311" s="12"/>
     </row>
-    <row r="312" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="312" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B312" s="7">
         <v>308</v>
       </c>
@@ -20649,7 +20685,7 @@
       </c>
       <c r="Y312" s="12"/>
     </row>
-    <row r="313" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="313" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B313" s="7">
         <v>309</v>
       </c>
@@ -20691,7 +20727,7 @@
       </c>
       <c r="Y313" s="12"/>
     </row>
-    <row r="314" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="314" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B314" s="7">
         <v>310</v>
       </c>
@@ -20731,7 +20767,7 @@
       </c>
       <c r="Y314" s="12"/>
     </row>
-    <row r="315" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="315" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B315" s="7">
         <v>311</v>
       </c>
@@ -20771,7 +20807,7 @@
       </c>
       <c r="Y315" s="12"/>
     </row>
-    <row r="316" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="316" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B316" s="7">
         <v>312</v>
       </c>
@@ -20811,7 +20847,7 @@
       </c>
       <c r="Y316" s="12"/>
     </row>
-    <row r="317" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="317" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B317" s="7">
         <v>313</v>
       </c>
@@ -20849,7 +20885,7 @@
       </c>
       <c r="Y317" s="12"/>
     </row>
-    <row r="318" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="318" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B318" s="7">
         <v>314</v>
       </c>
@@ -20887,7 +20923,7 @@
       </c>
       <c r="Y318" s="12"/>
     </row>
-    <row r="319" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="319" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B319" s="7">
         <v>315</v>
       </c>
@@ -20925,7 +20961,7 @@
       </c>
       <c r="Y319" s="12"/>
     </row>
-    <row r="320" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="320" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B320" s="7">
         <v>316</v>
       </c>
@@ -20965,7 +21001,7 @@
       </c>
       <c r="Y320" s="12"/>
     </row>
-    <row r="321" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="321" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B321" s="7">
         <v>317</v>
       </c>
@@ -21005,7 +21041,7 @@
       </c>
       <c r="Y321" s="12"/>
     </row>
-    <row r="322" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="322" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B322" s="7">
         <v>318</v>
       </c>
@@ -21045,7 +21081,7 @@
       </c>
       <c r="Y322" s="12"/>
     </row>
-    <row r="323" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="323" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B323" s="7">
         <v>319</v>
       </c>
@@ -21087,7 +21123,7 @@
       </c>
       <c r="Y323" s="12"/>
     </row>
-    <row r="324" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="324" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B324" s="7">
         <v>320</v>
       </c>
@@ -21129,7 +21165,7 @@
       </c>
       <c r="Y324" s="12"/>
     </row>
-    <row r="325" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="325" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B325" s="7">
         <v>321</v>
       </c>
@@ -21171,7 +21207,7 @@
       </c>
       <c r="Y325" s="12"/>
     </row>
-    <row r="326" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="326" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B326" s="7">
         <v>322</v>
       </c>
@@ -21217,7 +21253,7 @@
       </c>
       <c r="Y326" s="12"/>
     </row>
-    <row r="327" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="327" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B327" s="7">
         <v>323</v>
       </c>
@@ -21255,7 +21291,7 @@
       </c>
       <c r="Y327" s="12"/>
     </row>
-    <row r="328" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="328" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B328" s="7">
         <v>324</v>
       </c>
@@ -21297,7 +21333,7 @@
       </c>
       <c r="Y328" s="12"/>
     </row>
-    <row r="329" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="329" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B329" s="7">
         <v>325</v>
       </c>
@@ -21340,7 +21376,7 @@
       </c>
       <c r="Y329" s="12"/>
     </row>
-    <row r="330" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="330" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B330" s="7">
         <v>326</v>
       </c>
@@ -21383,7 +21419,7 @@
       <c r="X330" s="12"/>
       <c r="Y330" s="12"/>
     </row>
-    <row r="331" spans="2:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="2:25" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B331" s="7">
         <v>327</v>
       </c>
@@ -21424,7 +21460,7 @@
       <c r="X331" s="12"/>
       <c r="Y331" s="12"/>
     </row>
-    <row r="332" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="332" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B332" s="7">
         <v>328</v>
       </c>
@@ -21467,7 +21503,7 @@
       </c>
       <c r="Y332" s="12"/>
     </row>
-    <row r="333" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="333" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B333" s="7">
         <v>329</v>
       </c>
@@ -21510,7 +21546,7 @@
       </c>
       <c r="Y333" s="12"/>
     </row>
-    <row r="334" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="334" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B334" s="7">
         <v>330</v>
       </c>
@@ -21553,7 +21589,7 @@
       </c>
       <c r="Y334" s="12"/>
     </row>
-    <row r="335" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="335" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B335" s="7">
         <v>331</v>
       </c>
@@ -21600,7 +21636,7 @@
       </c>
       <c r="Y335" s="12"/>
     </row>
-    <row r="336" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="336" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B336" s="7">
         <v>332</v>
       </c>
@@ -21647,7 +21683,7 @@
       </c>
       <c r="Y336" s="12"/>
     </row>
-    <row r="337" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="337" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B337" s="7">
         <v>333</v>
       </c>
@@ -21694,7 +21730,7 @@
       </c>
       <c r="Y337" s="12"/>
     </row>
-    <row r="338" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="338" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B338" s="7">
         <v>334</v>
       </c>
@@ -21741,7 +21777,7 @@
       </c>
       <c r="Y338" s="12"/>
     </row>
-    <row r="339" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="339" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B339" s="7">
         <v>335</v>
       </c>
@@ -21788,7 +21824,7 @@
       </c>
       <c r="Y339" s="12"/>
     </row>
-    <row r="340" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="340" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B340" s="7">
         <v>336</v>
       </c>
@@ -21882,7 +21918,7 @@
       <c r="X341" s="12"/>
       <c r="Y341" s="12"/>
     </row>
-    <row r="342" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="342" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B342" s="7">
         <v>338</v>
       </c>
@@ -21976,7 +22012,7 @@
       <c r="X343" s="12"/>
       <c r="Y343" s="12"/>
     </row>
-    <row r="344" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="344" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B344" s="7">
         <v>340</v>
       </c>
@@ -22707,7 +22743,7 @@
       <c r="X358" s="12"/>
       <c r="Y358" s="12"/>
     </row>
-    <row r="359" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="359" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B359" s="7">
         <v>355</v>
       </c>
@@ -22850,7 +22886,7 @@
       <c r="X361" s="12"/>
       <c r="Y361" s="12"/>
     </row>
-    <row r="362" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="362" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B362" s="7">
         <v>358</v>
       </c>
@@ -22944,7 +22980,7 @@
       <c r="X363" s="12"/>
       <c r="Y363" s="12"/>
     </row>
-    <row r="364" spans="2:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="364" spans="2:25" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B364" s="7">
         <v>360</v>
       </c>
@@ -23136,7 +23172,7 @@
       <c r="X367" s="12"/>
       <c r="Y367" s="12"/>
     </row>
-    <row r="368" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="368" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B368" s="7">
         <v>364</v>
       </c>
@@ -23230,7 +23266,7 @@
       <c r="X369" s="12"/>
       <c r="Y369" s="12"/>
     </row>
-    <row r="370" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="370" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B370" s="7">
         <v>366</v>
       </c>
@@ -23373,7 +23409,7 @@
       <c r="X372" s="12"/>
       <c r="Y372" s="12"/>
     </row>
-    <row r="373" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="373" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B373" s="7">
         <v>369</v>
       </c>
@@ -23467,7 +23503,7 @@
       <c r="X374" s="12"/>
       <c r="Y374" s="12"/>
     </row>
-    <row r="375" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B375" s="7">
         <v>371</v>
       </c>
@@ -23514,7 +23550,7 @@
       </c>
       <c r="Y375" s="12"/>
     </row>
-    <row r="376" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="376" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B376" s="7">
         <v>372</v>
       </c>
@@ -23561,7 +23597,7 @@
       </c>
       <c r="Y376" s="12"/>
     </row>
-    <row r="377" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B377" s="7">
         <v>373</v>
       </c>
@@ -23606,7 +23642,7 @@
       <c r="X377" s="12"/>
       <c r="Y377" s="12"/>
     </row>
-    <row r="378" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="378" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B378" s="7">
         <v>374</v>
       </c>
@@ -23749,7 +23785,7 @@
       <c r="X380" s="12"/>
       <c r="Y380" s="12"/>
     </row>
-    <row r="381" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B381" s="7">
         <v>377</v>
       </c>
@@ -23892,7 +23928,7 @@
       <c r="X383" s="12"/>
       <c r="Y383" s="12"/>
     </row>
-    <row r="384" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B384" s="7">
         <v>380</v>
       </c>
@@ -23937,7 +23973,7 @@
       <c r="X384" s="12"/>
       <c r="Y384" s="12"/>
     </row>
-    <row r="385" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="385" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B385" s="7">
         <v>381</v>
       </c>
@@ -24080,7 +24116,7 @@
       <c r="X387" s="12"/>
       <c r="Y387" s="12"/>
     </row>
-    <row r="388" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="388" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B388" s="7">
         <v>384</v>
       </c>
@@ -24125,7 +24161,7 @@
       <c r="X388" s="12"/>
       <c r="Y388" s="12"/>
     </row>
-    <row r="389" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="389" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B389" s="7">
         <v>385</v>
       </c>
@@ -24219,7 +24255,7 @@
       <c r="X390" s="12"/>
       <c r="Y390" s="12"/>
     </row>
-    <row r="391" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="391" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B391" s="7">
         <v>387</v>
       </c>
@@ -24313,7 +24349,7 @@
       <c r="X392" s="12"/>
       <c r="Y392" s="12"/>
     </row>
-    <row r="393" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="393" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B393" s="7">
         <v>389</v>
       </c>
@@ -24358,7 +24394,7 @@
       <c r="X393" s="12"/>
       <c r="Y393" s="12"/>
     </row>
-    <row r="394" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="394" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B394" s="7">
         <v>390</v>
       </c>
@@ -24452,7 +24488,7 @@
       <c r="X395" s="12"/>
       <c r="Y395" s="12"/>
     </row>
-    <row r="396" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="396" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B396" s="7">
         <v>392</v>
       </c>
@@ -24595,7 +24631,7 @@
       <c r="X398" s="12"/>
       <c r="Y398" s="12"/>
     </row>
-    <row r="399" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="399" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B399" s="7">
         <v>395</v>
       </c>
@@ -24642,7 +24678,7 @@
       </c>
       <c r="Y399" s="12"/>
     </row>
-    <row r="400" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="400" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B400" s="7">
         <v>396</v>
       </c>
@@ -24689,7 +24725,7 @@
       </c>
       <c r="Y400" s="12"/>
     </row>
-    <row r="401" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="401" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B401" s="7">
         <v>397</v>
       </c>
@@ -24734,7 +24770,7 @@
       <c r="X401" s="12"/>
       <c r="Y401" s="12"/>
     </row>
-    <row r="402" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="402" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B402" s="7">
         <v>398</v>
       </c>
@@ -24781,7 +24817,7 @@
       </c>
       <c r="Y402" s="12"/>
     </row>
-    <row r="403" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="403" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B403" s="7">
         <v>399</v>
       </c>
@@ -24875,7 +24911,7 @@
       <c r="X404" s="12"/>
       <c r="Y404" s="12"/>
     </row>
-    <row r="405" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="405" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B405" s="7">
         <v>401</v>
       </c>
@@ -24920,7 +24956,7 @@
       <c r="X405" s="12"/>
       <c r="Y405" s="12"/>
     </row>
-    <row r="406" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="406" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B406" s="7">
         <v>402</v>
       </c>
@@ -25014,7 +25050,7 @@
       <c r="X407" s="12"/>
       <c r="Y407" s="12"/>
     </row>
-    <row r="408" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="408" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B408" s="7">
         <v>404</v>
       </c>
@@ -25157,7 +25193,7 @@
       <c r="X410" s="12"/>
       <c r="Y410" s="12"/>
     </row>
-    <row r="411" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="411" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B411" s="7">
         <v>407</v>
       </c>
@@ -25253,7 +25289,7 @@
       <c r="X412" s="12"/>
       <c r="Y412" s="12"/>
     </row>
-    <row r="413" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="413" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B413" s="7">
         <v>409</v>
       </c>
@@ -25349,7 +25385,7 @@
       <c r="X414" s="12"/>
       <c r="Y414" s="12"/>
     </row>
-    <row r="415" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="415" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B415" s="7">
         <v>411</v>
       </c>
@@ -25443,7 +25479,7 @@
       <c r="X416" s="12"/>
       <c r="Y416" s="12"/>
     </row>
-    <row r="417" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="417" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B417" s="7">
         <v>413</v>
       </c>
@@ -25586,7 +25622,7 @@
       <c r="X419" s="12"/>
       <c r="Y419" s="12"/>
     </row>
-    <row r="420" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="420" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B420" s="7">
         <v>416</v>
       </c>
@@ -25729,7 +25765,7 @@
       <c r="X422" s="12"/>
       <c r="Y422" s="12"/>
     </row>
-    <row r="423" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="423" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B423" s="7">
         <v>419</v>
       </c>
@@ -25774,7 +25810,7 @@
       <c r="X423" s="12"/>
       <c r="Y423" s="12"/>
     </row>
-    <row r="424" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="424" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B424" s="7">
         <v>420</v>
       </c>
@@ -26113,7 +26149,7 @@
       <c r="X430" s="12"/>
       <c r="Y430" s="12"/>
     </row>
-    <row r="431" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="431" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B431" s="7">
         <v>427</v>
       </c>
@@ -26407,7 +26443,7 @@
       <c r="X436" s="12"/>
       <c r="Y436" s="12"/>
     </row>
-    <row r="437" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="437" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B437" s="7">
         <v>433</v>
       </c>
@@ -26454,7 +26490,7 @@
       </c>
       <c r="Y437" s="12"/>
     </row>
-    <row r="438" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="438" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B438" s="7">
         <v>434</v>
       </c>
@@ -26746,7 +26782,7 @@
       <c r="X443" s="12"/>
       <c r="Y443" s="12"/>
     </row>
-    <row r="444" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="444" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B444" s="7">
         <v>440</v>
       </c>
@@ -26791,7 +26827,7 @@
       <c r="X444" s="12"/>
       <c r="Y444" s="12"/>
     </row>
-    <row r="445" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="445" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B445" s="7">
         <v>441</v>
       </c>
@@ -26836,7 +26872,7 @@
       <c r="X445" s="12"/>
       <c r="Y445" s="12"/>
     </row>
-    <row r="446" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="446" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B446" s="7">
         <v>442</v>
       </c>
@@ -26883,7 +26919,7 @@
       </c>
       <c r="Y446" s="12"/>
     </row>
-    <row r="447" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="447" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B447" s="7">
         <v>443</v>
       </c>
@@ -26979,7 +27015,7 @@
       <c r="X448" s="12"/>
       <c r="Y448" s="12"/>
     </row>
-    <row r="449" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="449" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B449" s="7">
         <v>445</v>
       </c>
@@ -27073,7 +27109,7 @@
       <c r="X450" s="12"/>
       <c r="Y450" s="12"/>
     </row>
-    <row r="451" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="451" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B451" s="7">
         <v>447</v>
       </c>
@@ -27120,7 +27156,7 @@
       </c>
       <c r="Y451" s="12"/>
     </row>
-    <row r="452" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="452" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B452" s="7">
         <v>448</v>
       </c>
@@ -27167,7 +27203,7 @@
       </c>
       <c r="Y452" s="12"/>
     </row>
-    <row r="453" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="453" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B453" s="7">
         <v>449</v>
       </c>
@@ -27214,7 +27250,7 @@
       </c>
       <c r="Y453" s="12"/>
     </row>
-    <row r="454" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="454" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B454" s="7">
         <v>450</v>
       </c>
@@ -27310,7 +27346,7 @@
       <c r="X455" s="12"/>
       <c r="Y455" s="12"/>
     </row>
-    <row r="456" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="456" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B456" s="7">
         <v>452</v>
       </c>
@@ -27357,7 +27393,7 @@
       </c>
       <c r="Y456" s="12"/>
     </row>
-    <row r="457" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="457" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B457" s="7">
         <v>453</v>
       </c>
@@ -27402,7 +27438,7 @@
       <c r="X457" s="12"/>
       <c r="Y457" s="12"/>
     </row>
-    <row r="458" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="458" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B458" s="7">
         <v>454</v>
       </c>
@@ -27447,7 +27483,7 @@
       <c r="X458" s="12"/>
       <c r="Y458" s="12"/>
     </row>
-    <row r="459" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="459" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B459" s="7">
         <v>455</v>
       </c>
@@ -27492,7 +27528,7 @@
       <c r="X459" s="12"/>
       <c r="Y459" s="12"/>
     </row>
-    <row r="460" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="460" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B460" s="7">
         <v>456</v>
       </c>
@@ -27537,7 +27573,7 @@
       <c r="X460" s="12"/>
       <c r="Y460" s="12"/>
     </row>
-    <row r="461" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="461" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B461" s="7">
         <v>457</v>
       </c>
@@ -27582,7 +27618,7 @@
       <c r="X461" s="12"/>
       <c r="Y461" s="12"/>
     </row>
-    <row r="462" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="462" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B462" s="7">
         <v>458</v>
       </c>
@@ -28754,7 +28790,7 @@
       <c r="X485" s="12"/>
       <c r="Y485" s="12"/>
     </row>
-    <row r="486" spans="2:25" ht="58" x14ac:dyDescent="0.35">
+    <row r="486" spans="2:25" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B486" s="7">
         <v>482</v>
       </c>
@@ -28799,7 +28835,7 @@
       <c r="X486" s="12"/>
       <c r="Y486" s="12"/>
     </row>
-    <row r="487" spans="2:25" ht="58" x14ac:dyDescent="0.35">
+    <row r="487" spans="2:25" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B487" s="7">
         <v>483</v>
       </c>
@@ -29089,7 +29125,7 @@
       <c r="X492" s="12"/>
       <c r="Y492" s="12"/>
     </row>
-    <row r="493" spans="2:25" ht="58" x14ac:dyDescent="0.35">
+    <row r="493" spans="2:25" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B493" s="7">
         <v>489</v>
       </c>
@@ -29134,7 +29170,7 @@
       <c r="X493" s="12"/>
       <c r="Y493" s="12"/>
     </row>
-    <row r="494" spans="2:25" ht="58" x14ac:dyDescent="0.35">
+    <row r="494" spans="2:25" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B494" s="7">
         <v>490</v>
       </c>
@@ -29181,7 +29217,7 @@
       </c>
       <c r="Y494" s="12"/>
     </row>
-    <row r="495" spans="2:25" ht="58" x14ac:dyDescent="0.35">
+    <row r="495" spans="2:25" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B495" s="7">
         <v>491</v>
       </c>
@@ -29226,7 +29262,7 @@
       <c r="X495" s="12"/>
       <c r="Y495" s="12"/>
     </row>
-    <row r="496" spans="2:25" ht="58" x14ac:dyDescent="0.35">
+    <row r="496" spans="2:25" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="B496" s="7">
         <v>492</v>
       </c>
@@ -29271,7 +29307,7 @@
       <c r="X496" s="12"/>
       <c r="Y496" s="12"/>
     </row>
-    <row r="497" spans="2:25" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="497" spans="2:25" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B497" s="7">
         <v>493</v>
       </c>
@@ -29804,7 +29840,7 @@
       <c r="X507" s="13"/>
       <c r="Y507" s="13"/>
     </row>
-    <row r="508" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="508" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B508" s="7">
         <v>504</v>
       </c>
@@ -29847,7 +29883,7 @@
       <c r="X508" s="12"/>
       <c r="Y508" s="12"/>
     </row>
-    <row r="509" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="509" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B509" s="7">
         <v>505</v>
       </c>
@@ -29888,7 +29924,7 @@
       <c r="X509" s="12"/>
       <c r="Y509" s="12"/>
     </row>
-    <row r="510" spans="2:25" ht="98" x14ac:dyDescent="0.35">
+    <row r="510" spans="2:25" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B510" s="7">
         <v>506</v>
       </c>
@@ -29935,7 +29971,7 @@
       <c r="X510" s="12"/>
       <c r="Y510" s="12"/>
     </row>
-    <row r="511" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="511" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B511" s="7">
         <v>507</v>
       </c>
@@ -29982,7 +30018,7 @@
       <c r="X511" s="12"/>
       <c r="Y511" s="12"/>
     </row>
-    <row r="512" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="512" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B512" s="7">
         <v>508</v>
       </c>
@@ -30029,7 +30065,7 @@
       <c r="X512" s="12"/>
       <c r="Y512" s="12"/>
     </row>
-    <row r="513" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="513" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B513" s="7">
         <v>509</v>
       </c>
@@ -30076,7 +30112,7 @@
       <c r="X513" s="12"/>
       <c r="Y513" s="12"/>
     </row>
-    <row r="514" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="514" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B514" s="7">
         <v>510</v>
       </c>
@@ -30123,7 +30159,7 @@
       <c r="X514" s="12"/>
       <c r="Y514" s="12"/>
     </row>
-    <row r="515" spans="2:25" ht="98" x14ac:dyDescent="0.35">
+    <row r="515" spans="2:25" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B515" s="7">
         <v>511</v>
       </c>
@@ -30170,7 +30206,7 @@
       <c r="X515" s="12"/>
       <c r="Y515" s="12"/>
     </row>
-    <row r="516" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="516" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B516" s="7">
         <v>512</v>
       </c>
@@ -30221,7 +30257,7 @@
       </c>
       <c r="Y516" s="12"/>
     </row>
-    <row r="517" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="517" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B517" s="7">
         <v>513</v>
       </c>
@@ -30272,7 +30308,7 @@
       </c>
       <c r="Y517" s="12"/>
     </row>
-    <row r="518" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="518" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B518" s="7">
         <v>514</v>
       </c>
@@ -30323,7 +30359,7 @@
       </c>
       <c r="Y518" s="12"/>
     </row>
-    <row r="519" spans="2:25" ht="84" x14ac:dyDescent="0.35">
+    <row r="519" spans="2:25" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="B519" s="7">
         <v>515</v>
       </c>
@@ -30374,7 +30410,7 @@
       </c>
       <c r="Y519" s="12"/>
     </row>
-    <row r="520" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="520" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B520" s="7">
         <v>516</v>
       </c>
@@ -30425,7 +30461,7 @@
       </c>
       <c r="Y520" s="12"/>
     </row>
-    <row r="521" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="521" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B521" s="7">
         <v>517</v>
       </c>
@@ -30476,7 +30512,7 @@
       </c>
       <c r="Y521" s="12"/>
     </row>
-    <row r="522" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="522" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B522" s="7">
         <v>518</v>
       </c>
@@ -30527,7 +30563,7 @@
       </c>
       <c r="Y522" s="12"/>
     </row>
-    <row r="523" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="523" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B523" s="7">
         <v>519</v>
       </c>
@@ -30578,7 +30614,7 @@
       </c>
       <c r="Y523" s="12"/>
     </row>
-    <row r="524" spans="2:25" ht="126" x14ac:dyDescent="0.35">
+    <row r="524" spans="2:25" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="B524" s="7">
         <v>520</v>
       </c>
@@ -30629,7 +30665,7 @@
       </c>
       <c r="Y524" s="12"/>
     </row>
-    <row r="525" spans="2:25" ht="98" x14ac:dyDescent="0.35">
+    <row r="525" spans="2:25" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="B525" s="7">
         <v>521</v>
       </c>
@@ -30680,7 +30716,7 @@
       </c>
       <c r="Y525" s="12"/>
     </row>
-    <row r="526" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="526" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B526" s="7">
         <v>522</v>
       </c>
@@ -30731,7 +30767,7 @@
       </c>
       <c r="Y526" s="12"/>
     </row>
-    <row r="527" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="527" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B527" s="7">
         <v>523</v>
       </c>
@@ -30782,7 +30818,7 @@
       </c>
       <c r="Y527" s="12"/>
     </row>
-    <row r="528" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="528" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B528" s="7">
         <v>524</v>
       </c>
@@ -30827,7 +30863,7 @@
       <c r="X528" s="13"/>
       <c r="Y528" s="13"/>
     </row>
-    <row r="529" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="529" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B529" s="7">
         <v>525</v>
       </c>
@@ -30876,7 +30912,7 @@
       </c>
       <c r="Y529" s="12"/>
     </row>
-    <row r="530" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="530" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B530" s="7">
         <v>526</v>
       </c>
@@ -30923,7 +30959,7 @@
       <c r="X530" s="19"/>
       <c r="Y530" s="12"/>
     </row>
-    <row r="531" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="531" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B531" s="7">
         <v>527</v>
       </c>
@@ -30972,7 +31008,7 @@
       </c>
       <c r="Y531" s="12"/>
     </row>
-    <row r="532" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="532" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B532" s="7">
         <v>528</v>
       </c>
@@ -31021,7 +31057,7 @@
       </c>
       <c r="Y532" s="12"/>
     </row>
-    <row r="533" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="533" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B533" s="7">
         <v>529</v>
       </c>
@@ -31068,7 +31104,7 @@
       <c r="X533" s="12"/>
       <c r="Y533" s="12"/>
     </row>
-    <row r="534" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="534" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B534" s="7">
         <v>530</v>
       </c>
@@ -31115,7 +31151,7 @@
       <c r="X534" s="12"/>
       <c r="Y534" s="12"/>
     </row>
-    <row r="535" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="535" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B535" s="7">
         <v>531</v>
       </c>
@@ -31162,7 +31198,7 @@
       <c r="X535" s="12"/>
       <c r="Y535" s="12"/>
     </row>
-    <row r="536" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="536" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B536" s="7">
         <v>532</v>
       </c>
@@ -31209,7 +31245,7 @@
       <c r="X536" s="12"/>
       <c r="Y536" s="12"/>
     </row>
-    <row r="537" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="537" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B537" s="7">
         <v>533</v>
       </c>
@@ -31256,7 +31292,7 @@
       <c r="X537" s="12"/>
       <c r="Y537" s="12"/>
     </row>
-    <row r="538" spans="2:25" ht="70" x14ac:dyDescent="0.35">
+    <row r="538" spans="2:25" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="B538" s="7">
         <v>534</v>
       </c>
@@ -31303,7 +31339,7 @@
       <c r="X538" s="12"/>
       <c r="Y538" s="12"/>
     </row>
-    <row r="539" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="539" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B539" s="7">
         <v>535</v>
       </c>
@@ -31350,7 +31386,7 @@
       <c r="X539" s="12"/>
       <c r="Y539" s="12"/>
     </row>
-    <row r="540" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="540" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B540" s="7">
         <v>536</v>
       </c>
@@ -31399,7 +31435,7 @@
       </c>
       <c r="Y540" s="12"/>
     </row>
-    <row r="541" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="541" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B541" s="7">
         <v>537</v>
       </c>
@@ -31448,7 +31484,7 @@
       </c>
       <c r="Y541" s="12"/>
     </row>
-    <row r="542" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="542" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B542" s="7">
         <v>538</v>
       </c>
@@ -31497,7 +31533,7 @@
       </c>
       <c r="Y542" s="12"/>
     </row>
-    <row r="543" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="543" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B543" s="7">
         <v>539</v>
       </c>
@@ -31544,7 +31580,7 @@
       <c r="X543" s="12"/>
       <c r="Y543" s="12"/>
     </row>
-    <row r="544" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="544" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B544" s="7">
         <v>540</v>
       </c>
@@ -31591,7 +31627,7 @@
       <c r="X544" s="12"/>
       <c r="Y544" s="12"/>
     </row>
-    <row r="545" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="545" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B545" s="7">
         <v>541</v>
       </c>
@@ -31638,7 +31674,7 @@
       <c r="X545" s="12"/>
       <c r="Y545" s="12"/>
     </row>
-    <row r="546" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="546" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B546" s="7">
         <v>542</v>
       </c>
@@ -31687,7 +31723,7 @@
       </c>
       <c r="Y546" s="12"/>
     </row>
-    <row r="547" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="547" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B547" s="7">
         <v>543</v>
       </c>
@@ -31734,7 +31770,7 @@
       <c r="X547" s="12"/>
       <c r="Y547" s="12"/>
     </row>
-    <row r="548" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="548" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B548" s="7">
         <v>544</v>
       </c>
@@ -31781,7 +31817,7 @@
       <c r="X548" s="12"/>
       <c r="Y548" s="12"/>
     </row>
-    <row r="549" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="549" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B549" s="7">
         <v>545</v>
       </c>
@@ -31828,7 +31864,7 @@
       <c r="X549" s="12"/>
       <c r="Y549" s="12"/>
     </row>
-    <row r="550" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="550" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B550" s="7">
         <v>546</v>
       </c>
@@ -31875,7 +31911,7 @@
       <c r="X550" s="12"/>
       <c r="Y550" s="12"/>
     </row>
-    <row r="551" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="551" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B551" s="7">
         <v>547</v>
       </c>
@@ -31922,7 +31958,7 @@
       <c r="X551" s="12"/>
       <c r="Y551" s="12"/>
     </row>
-    <row r="552" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="552" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B552" s="7">
         <v>548</v>
       </c>
@@ -31969,7 +32005,7 @@
       <c r="X552" s="12"/>
       <c r="Y552" s="12"/>
     </row>
-    <row r="553" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="553" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B553" s="7">
         <v>549</v>
       </c>
@@ -32016,7 +32052,7 @@
       <c r="X553" s="12"/>
       <c r="Y553" s="12"/>
     </row>
-    <row r="554" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="554" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B554" s="7">
         <v>550</v>
       </c>
@@ -32063,7 +32099,7 @@
       <c r="X554" s="12"/>
       <c r="Y554" s="12"/>
     </row>
-    <row r="555" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="555" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B555" s="7">
         <v>551</v>
       </c>
@@ -32110,7 +32146,7 @@
       <c r="X555" s="12"/>
       <c r="Y555" s="12"/>
     </row>
-    <row r="556" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="556" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B556" s="7">
         <v>552</v>
       </c>
@@ -32157,7 +32193,7 @@
       <c r="X556" s="12"/>
       <c r="Y556" s="12"/>
     </row>
-    <row r="557" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="557" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B557" s="7">
         <v>553</v>
       </c>
@@ -32204,7 +32240,7 @@
       <c r="X557" s="12"/>
       <c r="Y557" s="12"/>
     </row>
-    <row r="558" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="558" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B558" s="7">
         <v>554</v>
       </c>
@@ -32251,7 +32287,7 @@
       <c r="X558" s="12"/>
       <c r="Y558" s="12"/>
     </row>
-    <row r="559" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="559" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B559" s="7">
         <v>555</v>
       </c>
@@ -32298,7 +32334,7 @@
       <c r="X559" s="12"/>
       <c r="Y559" s="12"/>
     </row>
-    <row r="560" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="560" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B560" s="7">
         <v>556</v>
       </c>
@@ -32345,7 +32381,7 @@
       <c r="X560" s="12"/>
       <c r="Y560" s="12"/>
     </row>
-    <row r="561" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="561" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B561" s="7">
         <v>557</v>
       </c>
@@ -32392,7 +32428,7 @@
       <c r="X561" s="12"/>
       <c r="Y561" s="12"/>
     </row>
-    <row r="562" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="562" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B562" s="7">
         <v>558</v>
       </c>
@@ -32439,7 +32475,7 @@
       <c r="X562" s="12"/>
       <c r="Y562" s="12"/>
     </row>
-    <row r="563" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="563" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B563" s="7">
         <v>559</v>
       </c>
@@ -32486,7 +32522,7 @@
       <c r="X563" s="12"/>
       <c r="Y563" s="12"/>
     </row>
-    <row r="564" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="564" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B564" s="7">
         <v>560</v>
       </c>
@@ -32533,7 +32569,7 @@
       <c r="X564" s="12"/>
       <c r="Y564" s="12"/>
     </row>
-    <row r="565" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="565" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B565" s="7">
         <v>561</v>
       </c>
@@ -32580,7 +32616,7 @@
       <c r="X565" s="12"/>
       <c r="Y565" s="12"/>
     </row>
-    <row r="566" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="566" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B566" s="7">
         <v>562</v>
       </c>
@@ -32627,7 +32663,7 @@
       <c r="X566" s="12"/>
       <c r="Y566" s="12"/>
     </row>
-    <row r="567" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="567" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B567" s="7">
         <v>563</v>
       </c>
@@ -32674,7 +32710,7 @@
       <c r="X567" s="12"/>
       <c r="Y567" s="12"/>
     </row>
-    <row r="568" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="568" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B568" s="7">
         <v>564</v>
       </c>
@@ -32721,7 +32757,7 @@
       <c r="X568" s="12"/>
       <c r="Y568" s="12"/>
     </row>
-    <row r="569" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="569" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B569" s="7">
         <v>565</v>
       </c>
@@ -32768,7 +32804,7 @@
       <c r="X569" s="12"/>
       <c r="Y569" s="12"/>
     </row>
-    <row r="570" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="570" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B570" s="7">
         <v>566</v>
       </c>
@@ -32815,7 +32851,7 @@
       <c r="X570" s="12"/>
       <c r="Y570" s="12"/>
     </row>
-    <row r="571" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="571" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B571" s="7">
         <v>567</v>
       </c>
@@ -32862,7 +32898,7 @@
       <c r="X571" s="12"/>
       <c r="Y571" s="12"/>
     </row>
-    <row r="572" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="572" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B572" s="7">
         <v>568</v>
       </c>
@@ -32911,7 +32947,7 @@
       </c>
       <c r="Y572" s="12"/>
     </row>
-    <row r="573" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="573" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B573" s="7">
         <v>569</v>
       </c>
@@ -32958,7 +32994,7 @@
       <c r="X573" s="12"/>
       <c r="Y573" s="12"/>
     </row>
-    <row r="574" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="574" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B574" s="7">
         <v>570</v>
       </c>
@@ -33005,7 +33041,7 @@
       <c r="X574" s="12"/>
       <c r="Y574" s="12"/>
     </row>
-    <row r="575" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="575" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B575" s="7">
         <v>571</v>
       </c>
@@ -33052,7 +33088,7 @@
       <c r="X575" s="12"/>
       <c r="Y575" s="12"/>
     </row>
-    <row r="576" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="576" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B576" s="7">
         <v>572</v>
       </c>
@@ -33101,7 +33137,7 @@
       </c>
       <c r="Y576" s="12"/>
     </row>
-    <row r="577" spans="2:25" ht="56" x14ac:dyDescent="0.35">
+    <row r="577" spans="2:25" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B577" s="7">
         <v>573</v>
       </c>
@@ -33148,7 +33184,7 @@
       <c r="X577" s="12"/>
       <c r="Y577" s="12"/>
     </row>
-    <row r="578" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="578" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B578" s="7">
         <v>574</v>
       </c>
@@ -33195,7 +33231,7 @@
       <c r="X578" s="12"/>
       <c r="Y578" s="12"/>
     </row>
-    <row r="579" spans="2:25" ht="28" x14ac:dyDescent="0.35">
+    <row r="579" spans="2:25" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="B579" s="7">
         <v>575</v>
       </c>
@@ -33242,7 +33278,7 @@
       <c r="X579" s="12"/>
       <c r="Y579" s="12"/>
     </row>
-    <row r="580" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="580" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B580" s="7">
         <v>576</v>
       </c>
@@ -33289,7 +33325,7 @@
       <c r="X580" s="12"/>
       <c r="Y580" s="12"/>
     </row>
-    <row r="581" spans="2:25" ht="42" x14ac:dyDescent="0.35">
+    <row r="581" spans="2:25" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B581" s="7">
         <v>577</v>
       </c>
@@ -33334,7 +33370,7 @@
       <c r="X581" s="13"/>
       <c r="Y581" s="13"/>
     </row>
-    <row r="582" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="582" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B582" s="7">
         <v>578</v>
       </c>
@@ -33371,7 +33407,7 @@
       <c r="X582" s="9"/>
       <c r="Y582" s="9"/>
     </row>
-    <row r="583" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="583" spans="2:25" hidden="1" x14ac:dyDescent="0.35">
       <c r="B583" s="7">
         <v>579</v>
       </c>
@@ -33408,6 +33444,7 @@
       <c r="X583" s="9"/>
       <c r="Y583" s="9"/>
     </row>
+    <row r="584" spans="2:25" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="585" spans="2:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="586" spans="2:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I586" s="26" t="s">
@@ -33419,11 +33456,24 @@
       <c r="M586" s="27"/>
       <c r="N586" s="27">
         <f>SUM(N5:N583)</f>
-        <v>4358.45</v>
+        <v>4768.4499999999935</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:Y584" xr:uid="{CD8246AE-DFCC-4B3F-9CC4-F6A1FFD84A0B}"/>
+  <autoFilter ref="B4:Y584" xr:uid="{CD8246AE-DFCC-4B3F-9CC4-F6A1FFD84A0B}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Real Biometrics Release - Additional"/>
+        <filter val="Real Biometrics Release - Integration"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Vital"/>
+        <filter val="Vital?"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="D89:D90"/>
     <mergeCell ref="B2:D2"/>

</xml_diff>

<commit_message>
updated Reg Client estimates
</commit_message>
<xml_diff>
--- a/_files/requirements/MOSIP_Backlog_Consolidated.xlsx
+++ b/_files/requirements/MOSIP_Backlog_Consolidated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BEFAB9-4578-4EA6-83DA-C307CC4CF52E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02DCCF0-3C79-45C4-ADE6-B22060D7A700}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4873" uniqueCount="1798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4874" uniqueCount="1799">
   <si>
     <t>MOSIP - Consolidated Roadmap post 30Jun</t>
   </si>
@@ -5946,6 +5946,9 @@
   </si>
   <si>
     <t>20 - all bio type integration.</t>
+  </si>
+  <si>
+    <t>MOS-28476</t>
   </si>
 </sst>
 </file>
@@ -6177,7 +6180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6292,6 +6295,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6300,12 +6312,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -21550,7 +21556,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:J8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="24">
     <pivotField showAll="0"/>
@@ -22195,10 +22201,10 @@
   <dimension ref="A1:AB586"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -22233,11 +22239,11 @@
   <sheetData>
     <row r="1" spans="2:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:28" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
       <c r="Z2" s="21"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.35">
@@ -23931,9 +23937,9 @@
         <v>620</v>
       </c>
       <c r="Y39" s="10"/>
-      <c r="Z39" s="43"/>
-      <c r="AA39" s="43"/>
-      <c r="AB39" s="43"/>
+      <c r="Z39" s="40"/>
+      <c r="AA39" s="40"/>
+      <c r="AB39" s="40"/>
     </row>
     <row r="40" spans="2:28" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="B40" s="7">
@@ -25812,7 +25818,7 @@
         <v>714</v>
       </c>
       <c r="N77" s="12">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="O77" s="12"/>
       <c r="P77" s="12"/>
@@ -26038,7 +26044,7 @@
         <v>721</v>
       </c>
       <c r="N81" s="12">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
@@ -26097,7 +26103,7 @@
         <v>721</v>
       </c>
       <c r="N82" s="12">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="O82" s="12"/>
       <c r="P82" s="12"/>
@@ -26453,7 +26459,7 @@
       <c r="C89" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D89" s="39" t="s">
+      <c r="D89" s="42" t="s">
         <v>154</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -26500,7 +26506,7 @@
       <c r="C90" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D90" s="39"/>
+      <c r="D90" s="42"/>
       <c r="E90" s="12" t="s">
         <v>18</v>
       </c>
@@ -29125,7 +29131,7 @@
         <v>343</v>
       </c>
       <c r="N142" s="12">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="O142" s="12"/>
       <c r="P142" s="12"/>
@@ -29164,7 +29170,9 @@
       <c r="F143" s="12" t="s">
         <v>796</v>
       </c>
-      <c r="G143" s="12"/>
+      <c r="G143" s="39" t="s">
+        <v>1798</v>
+      </c>
       <c r="H143" s="12" t="s">
         <v>797</v>
       </c>
@@ -29558,7 +29566,7 @@
       <c r="L150" s="13"/>
       <c r="M150" s="13"/>
       <c r="N150" s="13">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="O150" s="13"/>
       <c r="P150" s="13"/>
@@ -30418,7 +30426,7 @@
         <v>641</v>
       </c>
       <c r="AA167" s="9"/>
-      <c r="AB167" s="44" t="s">
+      <c r="AB167" s="41" t="s">
         <v>1781</v>
       </c>
     </row>
@@ -31704,7 +31712,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="192" spans="2:28" ht="56" x14ac:dyDescent="0.35">
+    <row r="192" spans="2:28" ht="42" x14ac:dyDescent="0.35">
       <c r="B192" s="7">
         <v>188</v>
       </c>
@@ -32368,7 +32376,7 @@
       </c>
       <c r="AB203" s="9"/>
     </row>
-    <row r="204" spans="2:28" ht="140" x14ac:dyDescent="0.35">
+    <row r="204" spans="2:28" ht="126" x14ac:dyDescent="0.35">
       <c r="B204" s="7">
         <v>200</v>
       </c>
@@ -32427,7 +32435,7 @@
       </c>
       <c r="AB204" s="9"/>
     </row>
-    <row r="205" spans="2:28" ht="140" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:28" ht="126" x14ac:dyDescent="0.35">
       <c r="B205" s="7">
         <v>201</v>
       </c>
@@ -34661,9 +34669,9 @@
         <v>1153</v>
       </c>
       <c r="Y246" s="10"/>
-      <c r="Z246" s="43"/>
-      <c r="AA246" s="43"/>
-      <c r="AB246" s="43"/>
+      <c r="Z246" s="40"/>
+      <c r="AA246" s="40"/>
+      <c r="AB246" s="40"/>
     </row>
     <row r="247" spans="2:28" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="B247" s="7">
@@ -34989,7 +34997,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="253" spans="2:28" ht="56" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:28" ht="42" x14ac:dyDescent="0.35">
       <c r="B253" s="7">
         <v>249</v>
       </c>
@@ -35482,9 +35490,9 @@
         <v>1184</v>
       </c>
       <c r="Y261" s="10"/>
-      <c r="Z261" s="43"/>
-      <c r="AA261" s="43"/>
-      <c r="AB261" s="43"/>
+      <c r="Z261" s="40"/>
+      <c r="AA261" s="40"/>
+      <c r="AB261" s="40"/>
     </row>
     <row r="262" spans="1:28" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" s="16"/>
@@ -40282,7 +40290,7 @@
       <c r="AA362" s="9"/>
       <c r="AB362" s="9"/>
     </row>
-    <row r="363" spans="2:28" ht="70" x14ac:dyDescent="0.35">
+    <row r="363" spans="2:28" ht="56" x14ac:dyDescent="0.35">
       <c r="B363" s="7">
         <v>359</v>
       </c>
@@ -40386,7 +40394,7 @@
       <c r="AA364" s="9"/>
       <c r="AB364" s="9"/>
     </row>
-    <row r="365" spans="2:28" ht="70" x14ac:dyDescent="0.35">
+    <row r="365" spans="2:28" ht="56" x14ac:dyDescent="0.35">
       <c r="B365" s="7">
         <v>361</v>
       </c>
@@ -51547,23 +51555,11 @@
       <c r="M586" s="27"/>
       <c r="N586" s="27">
         <f>SUM(N5:N583)</f>
-        <v>4923.4499999999953</v>
+        <v>4806.4499999999953</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A4:AA583" xr:uid="{DAF38173-2647-4D1D-AC29-7E2D7C79183F}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Admin"/>
-        <filter val="ID Authentication"/>
-        <filter val="ID-Authentication"/>
-        <filter val="ID-Repository"/>
-        <filter val="Kernel"/>
-        <filter val="Pre-registration"/>
-        <filter val="Registration Client"/>
-        <filter val="Registration Processor"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="0.9.5 - Additional"/>

</xml_diff>